<commit_message>
IO excel write +
</commit_message>
<xml_diff>
--- a/ExcelExampleWrite.xlsx
+++ b/ExcelExampleWrite.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Datatype</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>No fixed size</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>A</t>
@@ -108,7 +111,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -180,6 +183,50 @@
         <v>10</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B9" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -187,46 +234,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>